<commit_message>
WY allocation update - ben use fixes 02/05/2021.
WY allocation update - ben use fixes 02/05/2021.
</commit_message>
<xml_diff>
--- a/Wyoming/WaterAllocation/WY_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Wyoming/WaterAllocation/WY_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Wyoming\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0076056D-03F7-4AFD-A55B-3DABF1DCDCE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73797E3-5C17-4C2D-A946-C1C1C41D0D00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1692" windowWidth="23256" windowHeight="12576" tabRatio="714" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="7" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1343" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="511">
   <si>
     <t>Name</t>
   </si>
@@ -795,18 +795,6 @@
     <t>Wildlife</t>
   </si>
   <si>
-    <t>Industrial - ground water</t>
-  </si>
-  <si>
-    <t>Irrigation - ground water</t>
-  </si>
-  <si>
-    <t>Miscellaneous - ground water</t>
-  </si>
-  <si>
-    <t>Municipal - ground water</t>
-  </si>
-  <si>
     <t>Stock Watering</t>
   </si>
   <si>
@@ -825,15 +813,6 @@
     <t>Commercial</t>
   </si>
   <si>
-    <t>Maintain Natural Condition (Phase II Award)</t>
-  </si>
-  <si>
-    <t>Domestic - Surface water</t>
-  </si>
-  <si>
-    <t>Domestic (Phase II Award)</t>
-  </si>
-  <si>
     <t>Domestic Supply</t>
   </si>
   <si>
@@ -846,9 +825,6 @@
     <t>Fire Protection</t>
   </si>
   <si>
-    <t>Fish propagation</t>
-  </si>
-  <si>
     <t>Flood Control</t>
   </si>
   <si>
@@ -864,27 +840,6 @@
     <t>Ice Cutting</t>
   </si>
   <si>
-    <t>Instream Flow (Phase II Award)</t>
-  </si>
-  <si>
-    <t>Industrial - Surface water</t>
-  </si>
-  <si>
-    <t>Irrigation - Surface water</t>
-  </si>
-  <si>
-    <t>Instream Flow - Only State of Wyo can apply</t>
-  </si>
-  <si>
-    <t>Maintain Natural Lake Level (Phase II Award)</t>
-  </si>
-  <si>
-    <t>Municipal - Surface water</t>
-  </si>
-  <si>
-    <t>Natural Flow (Phase II Award)</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -906,18 +861,12 @@
     <t>Temporary</t>
   </si>
   <si>
-    <t>Total Enlargement for this application</t>
-  </si>
-  <si>
     <t>Transportation</t>
   </si>
   <si>
     <t>Utilities</t>
   </si>
   <si>
-    <t>Wild &amp; Scenic - only State of Wyo can apply</t>
-  </si>
-  <si>
     <t>Wetlands</t>
   </si>
   <si>
@@ -957,9 +906,6 @@
     <t>COM</t>
   </si>
   <si>
-    <t>CON</t>
-  </si>
-  <si>
     <t>DOM_SW</t>
   </si>
   <si>
@@ -1062,54 +1008,27 @@
     <t>CAG</t>
   </si>
   <si>
-    <t>Commercial agriculture</t>
-  </si>
-  <si>
     <t>DEW</t>
   </si>
   <si>
-    <t>Mine dewatering</t>
-  </si>
-  <si>
     <t>HWY</t>
   </si>
   <si>
-    <t>Highway construction</t>
-  </si>
-  <si>
     <t>LAW</t>
   </si>
   <si>
-    <t>Large scale landscape</t>
-  </si>
-  <si>
     <t>O&amp;G</t>
   </si>
   <si>
-    <t>Oil &amp; Gas well drilling</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
     <t>P&amp;S</t>
   </si>
   <si>
-    <t>Potable &amp; Sanitary Supply</t>
-  </si>
-  <si>
     <t>SDG</t>
   </si>
   <si>
-    <t>&gt; gpm for Domestic &amp;/or stock</t>
-  </si>
-  <si>
     <t>SWD</t>
   </si>
   <si>
-    <t>Subdivison, water districts, etc</t>
-  </si>
-  <si>
     <t>SWP</t>
   </si>
   <si>
@@ -1119,24 +1038,9 @@
     <t>WHL</t>
   </si>
   <si>
-    <t>Water hauls</t>
-  </si>
-  <si>
-    <t>Coal bed methane - ground water</t>
-  </si>
-  <si>
-    <t>Domestic - ground water</t>
-  </si>
-  <si>
-    <t>Monitor, Observation</t>
-  </si>
-  <si>
     <t>AESCNG</t>
   </si>
   <si>
-    <t>Coal bed natural gas</t>
-  </si>
-  <si>
     <t>AQU</t>
   </si>
   <si>
@@ -1191,9 +1095,6 @@
     <t>Other - Commercial</t>
   </si>
   <si>
-    <t>Stockyard (Pig, Cow, Chicken)</t>
-  </si>
-  <si>
     <t>AESFIS</t>
   </si>
   <si>
@@ -1203,12 +1104,6 @@
     <t>AESGWR</t>
   </si>
   <si>
-    <t>Ground Water Recharge (Aesthetics)e</t>
-  </si>
-  <si>
-    <t>Dewatering</t>
-  </si>
-  <si>
     <t>DRI</t>
   </si>
   <si>
@@ -1284,9 +1179,6 @@
     <t>SDU</t>
   </si>
   <si>
-    <t>Stock and/or Domestic</t>
-  </si>
-  <si>
     <t>AESREC</t>
   </si>
   <si>
@@ -1299,9 +1191,6 @@
     <t>Stock (Aesthetics)</t>
   </si>
   <si>
-    <t>Construction</t>
-  </si>
-  <si>
     <t>DTA</t>
   </si>
   <si>
@@ -1335,13 +1224,7 @@
     <t>STW</t>
   </si>
   <si>
-    <t>Stock watering</t>
-  </si>
-  <si>
     <t>TWR</t>
-  </si>
-  <si>
-    <t>Tree watering (non-commercial)</t>
   </si>
   <si>
     <t>WDR</t>
@@ -1625,6 +1508,96 @@
   </si>
   <si>
     <t>Active</t>
+  </si>
+  <si>
+    <t>Ground Water Recharge (Aesthetics)</t>
+  </si>
+  <si>
+    <t>Total Enlargement</t>
+  </si>
+  <si>
+    <t>Commercial Agriculture</t>
+  </si>
+  <si>
+    <t>Coal Bed Methane - Ground Water</t>
+  </si>
+  <si>
+    <t>Mine Dewatering</t>
+  </si>
+  <si>
+    <t>Domestic - Ground Water</t>
+  </si>
+  <si>
+    <t>Domestic - Surface Water</t>
+  </si>
+  <si>
+    <t>Domestic (Phase 2 Award)</t>
+  </si>
+  <si>
+    <t>Fish Propagation</t>
+  </si>
+  <si>
+    <t>Highway Construction</t>
+  </si>
+  <si>
+    <t>Instream Flow (Phase 2 Award)</t>
+  </si>
+  <si>
+    <t>Industrial - Ground Water</t>
+  </si>
+  <si>
+    <t>Industrial - Surface Water</t>
+  </si>
+  <si>
+    <t>Irrigation - Ground Water</t>
+  </si>
+  <si>
+    <t>Irrigation - Surface Water</t>
+  </si>
+  <si>
+    <t>Maintain Natural Lake Level (Phase 2 Award)</t>
+  </si>
+  <si>
+    <t>Large Scale Landscape</t>
+  </si>
+  <si>
+    <t>Miscellaneous - Ground Water</t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>Municipal - Ground Water</t>
+  </si>
+  <si>
+    <t>Municipal - Surface Water</t>
+  </si>
+  <si>
+    <t>Natural Flow (Phase 2 Award)</t>
+  </si>
+  <si>
+    <t>Oil and Gas Well Drilling</t>
+  </si>
+  <si>
+    <t>Potable and Sanitary Supply</t>
+  </si>
+  <si>
+    <t>Gpm For Domestic or Stock</t>
+  </si>
+  <si>
+    <t>Stock and Domestic</t>
+  </si>
+  <si>
+    <t>Subdivision</t>
+  </si>
+  <si>
+    <t>Tree Watering</t>
+  </si>
+  <si>
+    <t>Wild and Scenic</t>
+  </si>
+  <si>
+    <t>Water Hauls</t>
   </si>
 </sst>
 </file>
@@ -2457,7 +2430,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2750,9 +2723,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2830,7 +2800,38 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3142,8 +3143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7154D4B-C952-456C-B506-1C3DB2041E3D}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3165,15 +3166,15 @@
         <v>237</v>
       </c>
       <c r="B2" t="s">
-        <v>485</v>
+        <v>446</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="B4" s="110" t="s">
-        <v>517</v>
+      <c r="B4" s="109" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -3187,17 +3188,17 @@
         <v>242</v>
       </c>
       <c r="B17" t="s">
-        <v>473</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>480</v>
+        <v>441</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>482</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -3314,7 +3315,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="96" t="s">
-        <v>504</v>
+        <v>465</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>38</v>
@@ -3326,7 +3327,7 @@
         <v>38</v>
       </c>
       <c r="I4" s="78" t="s">
-        <v>474</v>
+        <v>435</v>
       </c>
       <c r="J4" s="79" t="s">
         <v>189</v>
@@ -3346,7 +3347,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>475</v>
+        <v>436</v>
       </c>
       <c r="F5" s="47" t="s">
         <v>38</v>
@@ -3378,7 +3379,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="47" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>38</v>
@@ -3410,7 +3411,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="47" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F7" s="47" t="s">
         <v>38</v>
@@ -3442,7 +3443,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="47" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>38</v>
@@ -3474,7 +3475,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="43" t="s">
-        <v>518</v>
+        <v>479</v>
       </c>
       <c r="F9" s="47" t="s">
         <v>38</v>
@@ -3504,7 +3505,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="43" t="s">
-        <v>477</v>
+        <v>438</v>
       </c>
       <c r="F10" s="47" t="s">
         <v>38</v>
@@ -3536,7 +3537,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="95" t="s">
-        <v>478</v>
+        <v>439</v>
       </c>
       <c r="F11" s="47" t="s">
         <v>38</v>
@@ -3568,7 +3569,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="43" t="s">
-        <v>477</v>
+        <v>438</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>38</v>
@@ -3702,8 +3703,8 @@
       <c r="D4" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="105" t="s">
-        <v>481</v>
+      <c r="E4" s="104" t="s">
+        <v>442</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>38</v>
@@ -3734,7 +3735,7 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="106">
+      <c r="E5" s="105">
         <v>1</v>
       </c>
       <c r="F5" s="16"/>
@@ -3762,8 +3763,8 @@
       <c r="D6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="106" t="s">
-        <v>483</v>
+      <c r="E6" s="105" t="s">
+        <v>444</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>38</v>
@@ -3794,7 +3795,7 @@
       <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="105" t="s">
         <v>110</v>
       </c>
       <c r="F7" s="47" t="s">
@@ -3826,7 +3827,7 @@
       <c r="D8" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="106" t="s">
+      <c r="E8" s="105" t="s">
         <v>113</v>
       </c>
       <c r="F8" s="47" t="s">
@@ -3858,7 +3859,7 @@
       <c r="D9" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="106" t="s">
+      <c r="E9" s="105" t="s">
         <v>114</v>
       </c>
       <c r="F9" s="47" t="s">
@@ -3890,7 +3891,7 @@
       <c r="D10" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="106">
+      <c r="E10" s="105">
         <v>11</v>
       </c>
       <c r="F10" s="47" t="s">
@@ -3922,7 +3923,7 @@
       <c r="D11" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="106" t="s">
+      <c r="E11" s="105" t="s">
         <v>112</v>
       </c>
       <c r="F11" s="47" t="s">
@@ -3954,8 +3955,8 @@
       <c r="D12" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="106" t="s">
-        <v>479</v>
+      <c r="E12" s="105" t="s">
+        <v>440</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>38</v>
@@ -3986,8 +3987,8 @@
       <c r="D13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="106" t="s">
-        <v>479</v>
+      <c r="E13" s="105" t="s">
+        <v>440</v>
       </c>
       <c r="F13" s="47" t="s">
         <v>38</v>
@@ -4122,7 +4123,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="41" t="s">
-        <v>484</v>
+        <v>445</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>38</v>
@@ -4153,8 +4154,8 @@
       <c r="D5" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="111" t="s">
-        <v>489</v>
+      <c r="E5" s="110" t="s">
+        <v>450</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>38</v>
@@ -4186,7 +4187,7 @@
         <v>38</v>
       </c>
       <c r="E6" s="46" t="s">
-        <v>488</v>
+        <v>449</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>38</v>
@@ -4217,8 +4218,8 @@
       <c r="D7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="107" t="s">
-        <v>490</v>
+      <c r="E7" s="106" t="s">
+        <v>451</v>
       </c>
       <c r="F7" s="47" t="s">
         <v>38</v>
@@ -4249,8 +4250,8 @@
       <c r="D8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="108" t="s">
-        <v>485</v>
+      <c r="E8" s="107" t="s">
+        <v>446</v>
       </c>
       <c r="F8" s="47" t="s">
         <v>38</v>
@@ -4282,7 +4283,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>487</v>
+        <v>448</v>
       </c>
       <c r="F9" s="47" t="s">
         <v>38</v>
@@ -4314,7 +4315,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>492</v>
+        <v>453</v>
       </c>
       <c r="F10" s="47" t="s">
         <v>38</v>
@@ -4345,8 +4346,8 @@
       <c r="D11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="111" t="s">
-        <v>486</v>
+      <c r="E11" s="110" t="s">
+        <v>447</v>
       </c>
       <c r="F11" s="47" t="s">
         <v>38</v>
@@ -4378,7 +4379,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>491</v>
+        <v>452</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>38</v>
@@ -4534,7 +4535,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="67" t="s">
-        <v>493</v>
+        <v>454</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>38</v>
@@ -4564,7 +4565,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F5" s="45" t="s">
         <v>38</v>
@@ -4594,7 +4595,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F6" s="45" t="s">
         <v>38</v>
@@ -4657,10 +4658,10 @@
         <v>38</v>
       </c>
       <c r="F8" s="43" t="s">
-        <v>498</v>
+        <v>459</v>
       </c>
       <c r="G8" s="49" t="s">
-        <v>502</v>
+        <v>463</v>
       </c>
       <c r="H8" s="85"/>
       <c r="I8" s="78" t="s">
@@ -4684,7 +4685,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>38</v>
@@ -4714,7 +4715,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>494</v>
+        <v>455</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>38</v>
@@ -4851,7 +4852,7 @@
         <v>38</v>
       </c>
       <c r="E4" s="67" t="s">
-        <v>501</v>
+        <v>462</v>
       </c>
       <c r="F4" s="62" t="s">
         <v>38</v>
@@ -4881,7 +4882,7 @@
         <v>38</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="F5" s="47" t="s">
         <v>38</v>
@@ -4911,7 +4912,7 @@
         <v>20</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>38</v>
@@ -4941,7 +4942,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F7" s="47" t="s">
         <v>38</v>
@@ -5001,7 +5002,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F9" s="47" t="s">
         <v>38</v>
@@ -5029,7 +5030,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F10" s="47" t="s">
         <v>38</v>
@@ -5059,7 +5060,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F11" s="47" t="s">
         <v>38</v>
@@ -5089,7 +5090,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F12" s="47" t="s">
         <v>38</v>
@@ -5122,10 +5123,10 @@
         <v>38</v>
       </c>
       <c r="F13" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>514</v>
+        <v>475</v>
       </c>
       <c r="H13" s="87"/>
       <c r="I13" s="82" t="s">
@@ -5152,10 +5153,10 @@
         <v>38</v>
       </c>
       <c r="F14" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G14" s="48" t="s">
-        <v>515</v>
+        <v>476</v>
       </c>
       <c r="H14" s="87"/>
       <c r="I14" s="82">
@@ -5179,7 +5180,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F15" s="47" t="s">
         <v>38</v>
@@ -5209,7 +5210,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F16" s="47" t="s">
         <v>38</v>
@@ -5268,10 +5269,10 @@
         <v>38</v>
       </c>
       <c r="F18" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G18" s="32" t="s">
-        <v>497</v>
+        <v>458</v>
       </c>
       <c r="H18" s="83"/>
       <c r="I18" s="82" t="s">
@@ -5295,7 +5296,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>495</v>
+        <v>456</v>
       </c>
       <c r="F19" s="47" t="s">
         <v>38</v>
@@ -5325,7 +5326,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F20" s="47" t="s">
         <v>38</v>
@@ -5358,10 +5359,10 @@
         <v>38</v>
       </c>
       <c r="F21" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>496</v>
+        <v>457</v>
       </c>
       <c r="H21" s="83"/>
       <c r="I21" s="82" t="s">
@@ -5385,7 +5386,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="24" t="s">
-        <v>491</v>
+        <v>452</v>
       </c>
       <c r="F22" s="47" t="s">
         <v>38</v>
@@ -5415,7 +5416,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F23" s="47" t="s">
         <v>38</v>
@@ -5702,7 +5703,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="69" t="s">
-        <v>504</v>
+        <v>465</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>38</v>
@@ -5734,7 +5735,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>484</v>
+        <v>445</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>38</v>
@@ -5766,7 +5767,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="43" t="s">
-        <v>506</v>
+        <v>467</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>38</v>
@@ -5798,7 +5799,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="69" t="s">
-        <v>481</v>
+        <v>442</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>38</v>
@@ -5830,7 +5831,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="71" t="s">
-        <v>505</v>
+        <v>466</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>38</v>
@@ -5862,7 +5863,7 @@
         <v>20</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>38</v>
@@ -5894,7 +5895,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>38</v>
@@ -5926,7 +5927,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>38</v>
@@ -5958,7 +5959,7 @@
         <v>20</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>38</v>
@@ -5990,7 +5991,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>38</v>
@@ -6022,7 +6023,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>38</v>
@@ -6054,7 +6055,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>38</v>
@@ -6086,7 +6087,7 @@
         <v>20</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>38</v>
@@ -6121,10 +6122,10 @@
         <v>38</v>
       </c>
       <c r="F22" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>510</v>
+        <v>471</v>
       </c>
       <c r="H22" s="90" t="s">
         <v>38</v>
@@ -6150,10 +6151,10 @@
         <v>20</v>
       </c>
       <c r="E23" s="24" t="s">
-        <v>519</v>
+        <v>480</v>
       </c>
       <c r="F23" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G23" s="32" t="s">
         <v>38</v>
@@ -6185,10 +6186,10 @@
         <v>38</v>
       </c>
       <c r="F24" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>500</v>
+        <v>461</v>
       </c>
       <c r="H24" s="90" t="s">
         <v>38</v>
@@ -6214,13 +6215,13 @@
         <v>38</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>499</v>
+        <v>460</v>
       </c>
       <c r="F25" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G25" s="49" t="s">
-        <v>509</v>
+        <v>470</v>
       </c>
       <c r="H25" s="90" t="s">
         <v>38</v>
@@ -6247,10 +6248,10 @@
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G26" s="49" t="s">
-        <v>511</v>
+        <v>472</v>
       </c>
       <c r="H26" s="90" t="s">
         <v>38</v>
@@ -6276,7 +6277,7 @@
         <v>20</v>
       </c>
       <c r="E27" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>38</v>
@@ -6308,7 +6309,7 @@
         <v>38</v>
       </c>
       <c r="E28" s="24" t="s">
-        <v>507</v>
+        <v>468</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>38</v>
@@ -6340,7 +6341,7 @@
         <v>38</v>
       </c>
       <c r="E29" s="24" t="s">
-        <v>508</v>
+        <v>469</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>38</v>
@@ -6375,10 +6376,10 @@
         <v>38</v>
       </c>
       <c r="F30" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>512</v>
+        <v>473</v>
       </c>
       <c r="H30" s="90" t="s">
         <v>38</v>
@@ -6404,7 +6405,7 @@
         <v>38</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>38</v>
@@ -6436,13 +6437,13 @@
         <v>38</v>
       </c>
       <c r="E32" s="73" t="s">
-        <v>472</v>
+        <v>433</v>
       </c>
       <c r="F32" s="43" t="s">
-        <v>503</v>
+        <v>464</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>513</v>
+        <v>474</v>
       </c>
       <c r="H32" s="90" t="s">
         <v>38</v>
@@ -6468,7 +6469,7 @@
         <v>38</v>
       </c>
       <c r="E33" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>38</v>
@@ -6500,7 +6501,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>38</v>
@@ -6532,7 +6533,7 @@
         <v>20</v>
       </c>
       <c r="E35" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>38</v>
@@ -6596,7 +6597,7 @@
         <v>38</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>38</v>
@@ -6654,7 +6655,7 @@
         <v>38</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>38</v>
@@ -6686,7 +6687,7 @@
         <v>38</v>
       </c>
       <c r="E40" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>38</v>
@@ -6716,7 +6717,7 @@
         <v>20</v>
       </c>
       <c r="E41" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>38</v>
@@ -6748,7 +6749,7 @@
         <v>38</v>
       </c>
       <c r="E42" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>38</v>
@@ -6780,7 +6781,7 @@
         <v>38</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F43" s="24" t="s">
         <v>38</v>
@@ -6812,7 +6813,7 @@
         <v>20</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>38</v>
@@ -6876,7 +6877,7 @@
         <v>38</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>476</v>
+        <v>437</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>38</v>
@@ -6906,10 +6907,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A68CD9-E6C8-4C1E-8A36-F76F66BA5935}">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6924,2083 +6925,1555 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
-        <v>440</v>
-      </c>
-      <c r="G1" s="104" t="s">
-        <v>471</v>
+      <c r="A1" s="99" t="s">
+        <v>401</v>
+      </c>
+      <c r="G1" s="103" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="101" t="s">
-        <v>338</v>
-      </c>
-      <c r="C2" s="109" t="s">
-        <v>516</v>
-      </c>
-      <c r="F2" s="101" t="s">
+      <c r="B2" s="100" t="s">
+        <v>320</v>
+      </c>
+      <c r="C2" s="108" t="s">
+        <v>477</v>
+      </c>
+      <c r="F2" s="100" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="101" t="s">
-        <v>338</v>
+      <c r="G2" s="100" t="s">
+        <v>320</v>
       </c>
       <c r="H2" s="98"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="102" t="s">
-        <v>363</v>
-      </c>
-      <c r="B3" s="102" t="s">
-        <v>364</v>
+      <c r="A3" s="101" t="s">
+        <v>332</v>
+      </c>
+      <c r="B3" s="101" t="s">
+        <v>255</v>
       </c>
       <c r="C3" s="42" t="str">
         <f>""""&amp;A3&amp;""""&amp;" : "&amp;""""&amp;B3&amp;""""&amp;","</f>
-        <v>"AESCNG" : "Coal bed natural gas",</v>
+        <v>"AESCNG" : "Coal Bed Natural Gas",</v>
       </c>
       <c r="D3" s="42"/>
-      <c r="F3" s="102" t="s">
-        <v>442</v>
-      </c>
-      <c r="G3" s="102" t="s">
-        <v>443</v>
+      <c r="E3" s="42"/>
+      <c r="F3" s="101" t="s">
+        <v>403</v>
+      </c>
+      <c r="G3" s="101" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="102" t="s">
-        <v>384</v>
-      </c>
-      <c r="B4" s="102" t="s">
-        <v>385</v>
+      <c r="A4" s="101" t="s">
+        <v>351</v>
+      </c>
+      <c r="B4" s="101" t="s">
+        <v>352</v>
       </c>
       <c r="C4" s="42" t="str">
-        <f t="shared" ref="C4:C67" si="0">""""&amp;A4&amp;""""&amp;" : "&amp;""""&amp;B4&amp;""""&amp;","</f>
+        <f t="shared" ref="C4:C42" si="0">""""&amp;A4&amp;""""&amp;" : "&amp;""""&amp;B4&amp;""""&amp;","</f>
         <v>"AESFIS" : "Fish Propagation (Aesthetics)",</v>
       </c>
       <c r="D4" s="42"/>
-      <c r="F4" s="102" t="s">
-        <v>444</v>
-      </c>
-      <c r="G4" s="102" t="s">
-        <v>445</v>
+      <c r="E4" s="42"/>
+      <c r="F4" s="101" t="s">
+        <v>405</v>
+      </c>
+      <c r="G4" s="101" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="102" t="s">
-        <v>386</v>
-      </c>
-      <c r="B5" s="102" t="s">
-        <v>387</v>
+      <c r="A5" s="101" t="s">
+        <v>353</v>
+      </c>
+      <c r="B5" s="101" t="s">
+        <v>481</v>
       </c>
       <c r="C5" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"AESGWR" : "Ground Water Recharge (Aesthetics)e",</v>
+        <v>"AESGWR" : "Ground Water Recharge (Aesthetics)",</v>
       </c>
       <c r="D5" s="42"/>
-      <c r="F5" s="102" t="s">
-        <v>446</v>
-      </c>
-      <c r="G5" s="102" t="s">
-        <v>447</v>
+      <c r="E5" s="42"/>
+      <c r="F5" s="101" t="s">
+        <v>407</v>
+      </c>
+      <c r="G5" s="101" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="102" t="s">
-        <v>415</v>
-      </c>
-      <c r="B6" s="102" t="s">
-        <v>416</v>
+      <c r="A6" s="101" t="s">
+        <v>379</v>
+      </c>
+      <c r="B6" s="101" t="s">
+        <v>380</v>
       </c>
       <c r="C6" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"AESREC" : "Recreation (Aesthetics)",</v>
       </c>
       <c r="D6" s="42"/>
-      <c r="F6" s="102" t="s">
-        <v>448</v>
-      </c>
-      <c r="G6" s="102" t="s">
-        <v>449</v>
+      <c r="E6" s="42"/>
+      <c r="F6" s="101" t="s">
+        <v>409</v>
+      </c>
+      <c r="G6" s="101" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="102" t="s">
-        <v>417</v>
-      </c>
-      <c r="B7" s="102" t="s">
-        <v>418</v>
+      <c r="A7" s="101" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" s="101" t="s">
+        <v>382</v>
       </c>
       <c r="C7" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"AESSTK" : "Stock (Aesthetics)",</v>
       </c>
       <c r="D7" s="42"/>
-      <c r="F7" s="102" t="s">
-        <v>450</v>
-      </c>
-      <c r="G7" s="102" t="s">
-        <v>451</v>
+      <c r="E7" s="42"/>
+      <c r="F7" s="101" t="s">
+        <v>411</v>
+      </c>
+      <c r="G7" s="101" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="102" t="s">
-        <v>436</v>
-      </c>
-      <c r="B8" s="102" t="s">
-        <v>437</v>
+      <c r="A8" s="101" t="s">
+        <v>397</v>
+      </c>
+      <c r="B8" s="101" t="s">
+        <v>398</v>
       </c>
       <c r="C8" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"AESWET" : "Wetlands (Aesthetics)",</v>
       </c>
       <c r="D8" s="42"/>
-      <c r="F8" s="102" t="s">
-        <v>452</v>
-      </c>
-      <c r="G8" s="102" t="s">
-        <v>453</v>
+      <c r="E8" s="42"/>
+      <c r="F8" s="101" t="s">
+        <v>413</v>
+      </c>
+      <c r="G8" s="101" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="102" t="s">
-        <v>438</v>
-      </c>
-      <c r="B9" s="102" t="s">
-        <v>439</v>
+      <c r="A9" s="101" t="s">
+        <v>399</v>
+      </c>
+      <c r="B9" s="101" t="s">
+        <v>400</v>
       </c>
       <c r="C9" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"AESWIL" : "Wildlife (Aesthetics)",</v>
       </c>
       <c r="D9" s="42"/>
-      <c r="F9" s="102" t="s">
-        <v>454</v>
-      </c>
-      <c r="G9" s="102" t="s">
-        <v>455</v>
+      <c r="E9" s="42"/>
+      <c r="F9" s="101" t="s">
+        <v>415</v>
+      </c>
+      <c r="G9" s="101" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="102" t="s">
-        <v>365</v>
-      </c>
-      <c r="B10" s="102" t="s">
-        <v>366</v>
+      <c r="A10" s="101" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="101" t="s">
+        <v>334</v>
       </c>
       <c r="C10" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"AQU" : "Aquaculture",</v>
       </c>
       <c r="D10" s="42"/>
-      <c r="F10" s="102" t="s">
-        <v>456</v>
-      </c>
-      <c r="G10" s="102" t="s">
-        <v>457</v>
+      <c r="E10" s="42"/>
+      <c r="F10" s="101" t="s">
+        <v>417</v>
+      </c>
+      <c r="G10" s="101" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="102" t="s">
-        <v>367</v>
-      </c>
-      <c r="B11" s="102" t="s">
-        <v>368</v>
+      <c r="A11" s="101" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="101" t="s">
+        <v>336</v>
       </c>
       <c r="C11" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"BOT" : "Bottling Water",</v>
       </c>
       <c r="D11" s="42"/>
-      <c r="F11" s="102" t="s">
-        <v>458</v>
-      </c>
-      <c r="G11" s="102" t="s">
-        <v>459</v>
+      <c r="E11" s="42"/>
+      <c r="F11" s="101" t="s">
+        <v>419</v>
+      </c>
+      <c r="G11" s="101" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="102" t="s">
-        <v>339</v>
-      </c>
-      <c r="B12" s="102" t="s">
-        <v>340</v>
+      <c r="A12" s="101" t="s">
+        <v>321</v>
+      </c>
+      <c r="B12" s="101" t="s">
+        <v>483</v>
       </c>
       <c r="C12" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"CAG" : "Commercial agriculture",</v>
+        <v>"CAG" : "Commercial Agriculture",</v>
       </c>
       <c r="D12" s="42"/>
-      <c r="F12" s="102" t="s">
-        <v>460</v>
-      </c>
-      <c r="G12" s="102" t="s">
-        <v>461</v>
+      <c r="E12" s="42"/>
+      <c r="F12" s="101" t="s">
+        <v>421</v>
+      </c>
+      <c r="G12" s="101" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="102" t="s">
-        <v>293</v>
-      </c>
-      <c r="B13" s="102" t="s">
-        <v>360</v>
+      <c r="A13" s="101" t="s">
+        <v>276</v>
+      </c>
+      <c r="B13" s="101" t="s">
+        <v>484</v>
       </c>
       <c r="C13" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"CBM" : "Coal bed methane - ground water",</v>
+        <v>"CBM" : "Coal Bed Methane - Ground Water",</v>
       </c>
       <c r="D13" s="42"/>
-      <c r="F13" s="102" t="s">
+      <c r="E13" s="42"/>
+      <c r="F13" s="101" t="s">
         <v>138</v>
       </c>
-      <c r="G13" s="102" t="s">
-        <v>462</v>
+      <c r="G13" s="101" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="102" t="s">
-        <v>369</v>
-      </c>
-      <c r="B14" s="102" t="s">
-        <v>370</v>
+      <c r="A14" s="101" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="101" t="s">
+        <v>338</v>
       </c>
       <c r="C14" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"CHE" : "Chemical",</v>
       </c>
       <c r="D14" s="42"/>
-      <c r="F14" s="102" t="s">
-        <v>463</v>
-      </c>
-      <c r="G14" s="102" t="s">
-        <v>464</v>
+      <c r="E14" s="42"/>
+      <c r="F14" s="101" t="s">
+        <v>424</v>
+      </c>
+      <c r="G14" s="101" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="102" t="s">
-        <v>301</v>
-      </c>
-      <c r="B15" s="102" t="s">
-        <v>257</v>
+      <c r="A15" s="101" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="101" t="s">
+        <v>253</v>
       </c>
       <c r="C15" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"CIS" : "Consumptive Instream Flow",</v>
       </c>
       <c r="D15" s="42"/>
-      <c r="F15" s="102" t="s">
-        <v>465</v>
-      </c>
-      <c r="G15" s="102" t="s">
-        <v>466</v>
+      <c r="E15" s="42"/>
+      <c r="F15" s="101" t="s">
+        <v>426</v>
+      </c>
+      <c r="G15" s="101" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="102" t="s">
-        <v>302</v>
-      </c>
-      <c r="B16" s="102" t="s">
-        <v>258</v>
+      <c r="A16" s="101" t="s">
+        <v>285</v>
+      </c>
+      <c r="B16" s="101" t="s">
+        <v>254</v>
       </c>
       <c r="C16" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"CMU" : "Combined Uses",</v>
       </c>
       <c r="D16" s="42"/>
-      <c r="F16" s="102" t="s">
-        <v>467</v>
-      </c>
-      <c r="G16" s="102" t="s">
-        <v>468</v>
+      <c r="E16" s="42"/>
+      <c r="F16" s="101" t="s">
+        <v>428</v>
+      </c>
+      <c r="G16" s="101" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="102" t="s">
-        <v>303</v>
-      </c>
-      <c r="B17" s="102" t="s">
-        <v>259</v>
+      <c r="A17" s="101" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="101" t="s">
+        <v>255</v>
       </c>
       <c r="C17" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"CNG_SW" : "Coal Bed Natural Gas",</v>
       </c>
       <c r="D17" s="42"/>
-      <c r="F17" s="102" t="s">
-        <v>469</v>
-      </c>
-      <c r="G17" s="102" t="s">
-        <v>470</v>
+      <c r="E17" s="42"/>
+      <c r="F17" s="101" t="s">
+        <v>430</v>
+      </c>
+      <c r="G17" s="101" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B18" s="102" t="s">
-        <v>260</v>
+      <c r="A18" s="101" t="s">
+        <v>287</v>
+      </c>
+      <c r="B18" s="101" t="s">
+        <v>256</v>
       </c>
       <c r="C18" s="42" t="str">
         <f t="shared" si="0"/>
         <v>"COM" : "Commercial",</v>
       </c>
       <c r="D18" s="42"/>
-      <c r="F18" s="102" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="102" t="s">
+      <c r="E18" s="42"/>
+      <c r="F18" s="101" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="101" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B19" s="102" t="s">
-        <v>366</v>
+      <c r="A19" s="101" t="s">
+        <v>339</v>
+      </c>
+      <c r="B19" s="101" t="s">
+        <v>340</v>
       </c>
       <c r="C19" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Aquaculture",</v>
+        <v>"CUL" : "Culinary",</v>
       </c>
       <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B20" s="102" t="s">
-        <v>368</v>
+      <c r="A20" s="101" t="s">
+        <v>341</v>
+      </c>
+      <c r="B20" s="101" t="s">
+        <v>342</v>
       </c>
       <c r="C20" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Bottling Water",</v>
+        <v>"DAI" : "Dairy",</v>
       </c>
       <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B21" s="102" t="s">
-        <v>370</v>
+      <c r="A21" s="101" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" s="101" t="s">
+        <v>485</v>
       </c>
       <c r="C21" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Chemical",</v>
+        <v>"DEW" : "Mine Dewatering",</v>
       </c>
       <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B22" s="102" t="s">
-        <v>372</v>
+      <c r="A22" s="101" t="s">
+        <v>277</v>
+      </c>
+      <c r="B22" s="101" t="s">
+        <v>486</v>
       </c>
       <c r="C22" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Culinary",</v>
+        <v>"DOM_GW" : "Domestic - Ground Water",</v>
       </c>
       <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B23" s="102" t="s">
-        <v>374</v>
+      <c r="A23" s="101" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" s="101" t="s">
+        <v>487</v>
       </c>
       <c r="C23" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Dairy",</v>
+        <v>"DOM_SW" : "Domestic - Surface Water",</v>
       </c>
       <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B24" s="102" t="s">
-        <v>376</v>
+      <c r="A24" s="101" t="s">
+        <v>289</v>
+      </c>
+      <c r="B24" s="101" t="s">
+        <v>488</v>
       </c>
       <c r="C24" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Maintenance (Equipment Washing)",</v>
+        <v>"DPA" : "Domestic (Phase 2 Award)",</v>
       </c>
       <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B25" s="102" t="s">
-        <v>378</v>
+      <c r="A25" s="101" t="s">
+        <v>354</v>
+      </c>
+      <c r="B25" s="101" t="s">
+        <v>355</v>
       </c>
       <c r="C25" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Mechanical ",</v>
+        <v>"DRI" : "Drilling",</v>
       </c>
       <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B26" s="102" t="s">
-        <v>380</v>
+      <c r="A26" s="101" t="s">
+        <v>290</v>
+      </c>
+      <c r="B26" s="101" t="s">
+        <v>257</v>
       </c>
       <c r="C26" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Medicinal",</v>
+        <v>"DSP" : "Domestic Supply",</v>
       </c>
       <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B27" s="102" t="s">
-        <v>382</v>
+      <c r="A27" s="101" t="s">
+        <v>383</v>
+      </c>
+      <c r="B27" s="101" t="s">
+        <v>384</v>
       </c>
       <c r="C27" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Other - Commercial",</v>
+        <v>"DTA" : "Dust Abatement",</v>
       </c>
       <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="102" t="s">
-        <v>304</v>
-      </c>
-      <c r="B28" s="102" t="s">
-        <v>383</v>
+      <c r="A28" s="101" t="s">
+        <v>291</v>
+      </c>
+      <c r="B28" s="101" t="s">
+        <v>258</v>
       </c>
       <c r="C28" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"COM" : "Stockyard (Pig, Cow, Chicken)",</v>
+        <v>"ECAP" : "Existing Capacity",</v>
       </c>
       <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="B29" s="102" t="s">
-        <v>261</v>
+      <c r="A29" s="101" t="s">
+        <v>292</v>
+      </c>
+      <c r="B29" s="101" t="s">
+        <v>259</v>
       </c>
       <c r="C29" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"CON" : "Maintain Natural Condition (Phase II Award)",</v>
+        <v>"ERO" : "Erosion Control",</v>
       </c>
       <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="102" t="s">
-        <v>305</v>
-      </c>
-      <c r="B30" s="102" t="s">
-        <v>419</v>
+      <c r="A30" s="101" t="s">
+        <v>293</v>
+      </c>
+      <c r="B30" s="101" t="s">
+        <v>260</v>
       </c>
       <c r="C30" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"CON" : "Construction",</v>
+        <v>"FIR" : "Fire Protection",</v>
       </c>
       <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="102" t="s">
-        <v>371</v>
-      </c>
-      <c r="B31" s="102" t="s">
-        <v>372</v>
+      <c r="A31" s="101" t="s">
+        <v>294</v>
+      </c>
+      <c r="B31" s="101" t="s">
+        <v>489</v>
       </c>
       <c r="C31" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"CUL" : "Culinary",</v>
+        <v>"FIS" : "Fish Propagation",</v>
       </c>
       <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="102" t="s">
-        <v>373</v>
-      </c>
-      <c r="B32" s="102" t="s">
-        <v>374</v>
+      <c r="A32" s="101" t="s">
+        <v>295</v>
+      </c>
+      <c r="B32" s="101" t="s">
+        <v>261</v>
       </c>
       <c r="C32" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DAI" : "Dairy",</v>
+        <v>"FLO" : "Flood Control",</v>
       </c>
       <c r="D32" s="42"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="102" t="s">
-        <v>341</v>
-      </c>
-      <c r="B33" s="102" t="s">
-        <v>342</v>
+      <c r="E32" s="42"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="101" t="s">
+        <v>296</v>
+      </c>
+      <c r="B33" s="101" t="s">
+        <v>262</v>
       </c>
       <c r="C33" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DEW" : "Mine dewatering",</v>
+        <v>"FTH" : "Flow Through",</v>
       </c>
       <c r="D33" s="42"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102" t="s">
-        <v>341</v>
-      </c>
-      <c r="B34" s="102" t="s">
-        <v>388</v>
+      <c r="E33" s="42"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="101" t="s">
+        <v>297</v>
+      </c>
+      <c r="B34" s="101" t="s">
+        <v>263</v>
       </c>
       <c r="C34" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DEW" : "Dewatering",</v>
+        <v>"GWR" : "Ground Water Recharge",</v>
       </c>
       <c r="D34" s="42"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="102" t="s">
-        <v>294</v>
-      </c>
-      <c r="B35" s="102" t="s">
-        <v>361</v>
+      <c r="E34" s="42"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="101" t="s">
+        <v>356</v>
+      </c>
+      <c r="B35" s="101" t="s">
+        <v>357</v>
       </c>
       <c r="C35" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DOM_GW" : "Domestic - ground water",</v>
+        <v>"HEX" : "Heat Extraction",</v>
       </c>
       <c r="D35" s="42"/>
-    </row>
-    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="102" t="s">
-        <v>306</v>
-      </c>
-      <c r="B36" s="102" t="s">
-        <v>262</v>
+      <c r="E35" s="42"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="101" t="s">
+        <v>323</v>
+      </c>
+      <c r="B36" s="101" t="s">
+        <v>490</v>
       </c>
       <c r="C36" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DOM_SW" : "Domestic - Surface water",</v>
+        <v>"HWY" : "Highway Construction",</v>
       </c>
       <c r="D36" s="42"/>
-    </row>
-    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="102" t="s">
-        <v>307</v>
-      </c>
-      <c r="B37" s="102" t="s">
-        <v>263</v>
+      <c r="E36" s="42"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="101" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" s="101" t="s">
+        <v>264</v>
       </c>
       <c r="C37" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DPA" : "Domestic (Phase II Award)",</v>
+        <v>"HYD" : "Hydropower",</v>
       </c>
       <c r="D37" s="42"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="102" t="s">
-        <v>389</v>
-      </c>
-      <c r="B38" s="102" t="s">
-        <v>390</v>
+      <c r="E37" s="42"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="101" t="s">
+        <v>385</v>
+      </c>
+      <c r="B38" s="101" t="s">
+        <v>386</v>
       </c>
       <c r="C38" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DRI" : "Drilling",</v>
+        <v>"HYT" : "Hydrostatic Testing",</v>
       </c>
       <c r="D38" s="42"/>
-    </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="102" t="s">
-        <v>308</v>
-      </c>
-      <c r="B39" s="102" t="s">
-        <v>264</v>
+      <c r="E38" s="42"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="101" t="s">
+        <v>299</v>
+      </c>
+      <c r="B39" s="101" t="s">
+        <v>265</v>
       </c>
       <c r="C39" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DSP" : "Domestic Supply",</v>
+        <v>"ICE" : "Ice Cutting",</v>
       </c>
       <c r="D39" s="42"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="102" t="s">
-        <v>420</v>
-      </c>
-      <c r="B40" s="102" t="s">
-        <v>421</v>
+      <c r="E39" s="42"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="101" t="s">
+        <v>300</v>
+      </c>
+      <c r="B40" s="101" t="s">
+        <v>491</v>
       </c>
       <c r="C40" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"DTA" : "Dust Abatement",</v>
+        <v>"IFA" : "Instream Flow (Phase 2 Award)",</v>
       </c>
       <c r="D40" s="42"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="102" t="s">
-        <v>309</v>
-      </c>
-      <c r="B41" s="102" t="s">
-        <v>265</v>
+      <c r="E40" s="42"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="101" t="s">
+        <v>278</v>
+      </c>
+      <c r="B41" s="101" t="s">
+        <v>492</v>
       </c>
       <c r="C41" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"ECAP" : "Existing Capacity",</v>
+        <v>"IND_GW" : "Industrial - Ground Water",</v>
       </c>
       <c r="D41" s="42"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="102" t="s">
-        <v>310</v>
-      </c>
-      <c r="B42" s="102" t="s">
-        <v>266</v>
+      <c r="E41" s="42"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="101" t="s">
+        <v>301</v>
+      </c>
+      <c r="B42" s="101" t="s">
+        <v>493</v>
       </c>
       <c r="C42" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>"ERO" : "Erosion Control",</v>
+        <v>"IND_SW" : "Industrial - Surface Water",</v>
       </c>
       <c r="D42" s="42"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="102" t="s">
-        <v>311</v>
-      </c>
-      <c r="B43" s="102" t="s">
-        <v>267</v>
+      <c r="E42" s="42"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="101" t="s">
+        <v>279</v>
+      </c>
+      <c r="B43" s="101" t="s">
+        <v>494</v>
       </c>
       <c r="C43" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"FIR" : "Fire Protection",</v>
+        <f t="shared" ref="C43:C89" si="1">""""&amp;A43&amp;""""&amp;" : "&amp;""""&amp;B43&amp;""""&amp;","</f>
+        <v>"IRR_GW" : "Irrigation - Ground Water",</v>
       </c>
       <c r="D43" s="42"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="102" t="s">
-        <v>312</v>
-      </c>
-      <c r="B44" s="102" t="s">
-        <v>268</v>
+      <c r="E43" s="42"/>
+      <c r="G43" s="42"/>
+      <c r="H43"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="101" t="s">
+        <v>302</v>
+      </c>
+      <c r="B44" s="101" t="s">
+        <v>495</v>
       </c>
       <c r="C44" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"FIS" : "Fish propagation",</v>
+        <f t="shared" si="1"/>
+        <v>"IRR_SW" : "Irrigation - Surface Water",</v>
       </c>
       <c r="D44" s="42"/>
-    </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="102" t="s">
-        <v>312</v>
-      </c>
-      <c r="B45" s="102" t="s">
-        <v>385</v>
+      <c r="E44" s="42"/>
+      <c r="G44" s="42"/>
+      <c r="H44"/>
+    </row>
+    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="101" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" s="101" t="s">
+        <v>418</v>
       </c>
       <c r="C45" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"FIS" : "Fish Propagation (Aesthetics)",</v>
+        <f t="shared" si="1"/>
+        <v>"ISF" : "Instream Flow",</v>
       </c>
       <c r="D45" s="42"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="102" t="s">
-        <v>313</v>
-      </c>
-      <c r="B46" s="102" t="s">
-        <v>269</v>
+      <c r="E45" s="42"/>
+      <c r="G45" s="42"/>
+      <c r="H45"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="101" t="s">
+        <v>304</v>
+      </c>
+      <c r="B46" s="101" t="s">
+        <v>496</v>
       </c>
       <c r="C46" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"FLO" : "Flood Control",</v>
+        <f t="shared" si="1"/>
+        <v>"LAK" : "Maintain Natural Lake Level (Phase 2 Award)",</v>
       </c>
       <c r="D46" s="42"/>
-    </row>
-    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="102" t="s">
-        <v>314</v>
-      </c>
-      <c r="B47" s="102" t="s">
-        <v>270</v>
+      <c r="E46" s="42"/>
+      <c r="G46" s="42"/>
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="101" t="s">
+        <v>324</v>
+      </c>
+      <c r="B47" s="101" t="s">
+        <v>497</v>
       </c>
       <c r="C47" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"FTH" : "Flow Through",</v>
+        <f t="shared" si="1"/>
+        <v>"LAW" : "Large Scale Landscape",</v>
       </c>
       <c r="D47" s="42"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="102" t="s">
-        <v>315</v>
-      </c>
-      <c r="B48" s="102" t="s">
-        <v>271</v>
+      <c r="E47" s="42"/>
+      <c r="G47" s="42"/>
+      <c r="H47"/>
+    </row>
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="101" t="s">
+        <v>343</v>
+      </c>
+      <c r="B48" s="101" t="s">
+        <v>344</v>
       </c>
       <c r="C48" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"GWR" : "Ground Water Recharge",</v>
+        <f t="shared" si="1"/>
+        <v>"MAI" : "Maintenance (Equipment Washing)",</v>
       </c>
       <c r="D48" s="42"/>
+      <c r="E48" s="42"/>
+      <c r="G48" s="42"/>
+      <c r="H48"/>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="102" t="s">
-        <v>315</v>
-      </c>
-      <c r="B49" s="102" t="s">
+      <c r="A49" s="101" t="s">
+        <v>358</v>
+      </c>
+      <c r="B49" s="101" t="s">
+        <v>359</v>
+      </c>
+      <c r="C49" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>"MAN" : "Manufacturing",</v>
+      </c>
+      <c r="D49" s="42"/>
+      <c r="E49" s="42"/>
+      <c r="G49" s="42"/>
+      <c r="H49"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="101" t="s">
+        <v>345</v>
+      </c>
+      <c r="B50" s="101" t="s">
+        <v>346</v>
+      </c>
+      <c r="C50" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>"MEC" : "Mechanical ",</v>
+      </c>
+      <c r="D50" s="42"/>
+      <c r="E50" s="42"/>
+      <c r="G50" s="42"/>
+      <c r="H50"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="101" t="s">
+        <v>347</v>
+      </c>
+      <c r="B51" s="101" t="s">
+        <v>348</v>
+      </c>
+      <c r="C51" s="42" t="str">
+        <f t="shared" si="1"/>
+        <v>"MED" : "Medicinal",</v>
+      </c>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="101" t="s">
         <v>387</v>
       </c>
-      <c r="C49" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"GWR" : "Ground Water Recharge (Aesthetics)e",</v>
-      </c>
-      <c r="D49" s="42"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="102" t="s">
-        <v>391</v>
-      </c>
-      <c r="B50" s="102" t="s">
-        <v>392</v>
-      </c>
-      <c r="C50" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"HEX" : "Heat Extraction",</v>
-      </c>
-      <c r="D50" s="42"/>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="102" t="s">
-        <v>343</v>
-      </c>
-      <c r="B51" s="102" t="s">
-        <v>344</v>
-      </c>
-      <c r="C51" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"HWY" : "Highway construction",</v>
-      </c>
-      <c r="D51" s="42"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="102" t="s">
-        <v>316</v>
-      </c>
-      <c r="B52" s="102" t="s">
-        <v>272</v>
+      <c r="B52" s="101" t="s">
+        <v>388</v>
       </c>
       <c r="C52" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"HYD" : "Hydropower",</v>
+        <f t="shared" si="1"/>
+        <v>"MEM" : "Municipal (Emergency)",</v>
       </c>
       <c r="D52" s="42"/>
+      <c r="E52" s="42"/>
+      <c r="G52" s="42"/>
+      <c r="H52"/>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="102" t="s">
-        <v>422</v>
-      </c>
-      <c r="B53" s="102" t="s">
-        <v>423</v>
+      <c r="A53" s="101" t="s">
+        <v>360</v>
+      </c>
+      <c r="B53" s="101" t="s">
+        <v>361</v>
       </c>
       <c r="C53" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"HYT" : "Hydrostatic Testing",</v>
+        <f t="shared" si="1"/>
+        <v>"MIL" : "Milling",</v>
       </c>
       <c r="D53" s="42"/>
+      <c r="E53" s="42"/>
+      <c r="G53" s="42"/>
+      <c r="H53"/>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="102" t="s">
-        <v>317</v>
-      </c>
-      <c r="B54" s="102" t="s">
-        <v>273</v>
+      <c r="A54" s="101" t="s">
+        <v>362</v>
+      </c>
+      <c r="B54" s="101" t="s">
+        <v>363</v>
       </c>
       <c r="C54" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"ICE" : "Ice Cutting",</v>
+        <f t="shared" si="1"/>
+        <v>"MIN" : "Mining",</v>
       </c>
       <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54"/>
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="102" t="s">
-        <v>318</v>
-      </c>
-      <c r="B55" s="102" t="s">
-        <v>274</v>
+      <c r="A55" s="101" t="s">
+        <v>402</v>
+      </c>
+      <c r="B55" s="101" t="s">
+        <v>498</v>
       </c>
       <c r="C55" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IFA" : "Instream Flow (Phase II Award)",</v>
+        <f t="shared" si="1"/>
+        <v>"MIS" : "Miscellaneous - Ground Water",</v>
       </c>
       <c r="D55" s="42"/>
+      <c r="E55" s="42"/>
+      <c r="G55" s="42"/>
+      <c r="H55"/>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="102" t="s">
-        <v>295</v>
-      </c>
-      <c r="B56" s="102" t="s">
-        <v>251</v>
+      <c r="A56" s="101" t="s">
+        <v>280</v>
+      </c>
+      <c r="B56" s="101" t="s">
+        <v>499</v>
       </c>
       <c r="C56" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_GW" : "Industrial - ground water",</v>
+        <f t="shared" si="1"/>
+        <v>"MON" : "Monitor",</v>
       </c>
       <c r="D56" s="42"/>
+      <c r="E56" s="42"/>
+      <c r="G56" s="42"/>
+      <c r="H56"/>
     </row>
     <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B57" s="102" t="s">
-        <v>275</v>
+      <c r="A57" s="101" t="s">
+        <v>281</v>
+      </c>
+      <c r="B57" s="101" t="s">
+        <v>500</v>
       </c>
       <c r="C57" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Industrial - Surface water",</v>
+        <f t="shared" si="1"/>
+        <v>"MUN_GW" : "Municipal - Ground Water",</v>
       </c>
       <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57"/>
     </row>
     <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B58" s="102" t="s">
-        <v>388</v>
+      <c r="A58" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="B58" s="101" t="s">
+        <v>501</v>
       </c>
       <c r="C58" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Dewatering",</v>
+        <f t="shared" si="1"/>
+        <v>"MUN_SW" : "Municipal - Surface Water",</v>
       </c>
       <c r="D58" s="42"/>
+      <c r="E58" s="42"/>
+      <c r="G58" s="42"/>
+      <c r="H58"/>
     </row>
     <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B59" s="102" t="s">
-        <v>390</v>
+      <c r="A59" s="101" t="s">
+        <v>306</v>
+      </c>
+      <c r="B59" s="101" t="s">
+        <v>502</v>
       </c>
       <c r="C59" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Drilling",</v>
+        <f t="shared" si="1"/>
+        <v>"NAT" : "Natural Flow (Phase 2 Award)",</v>
       </c>
       <c r="D59" s="42"/>
+      <c r="E59" s="42"/>
+      <c r="G59" s="42"/>
+      <c r="H59"/>
     </row>
     <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B60" s="102" t="s">
-        <v>392</v>
+      <c r="A60" s="101" t="s">
+        <v>325</v>
+      </c>
+      <c r="B60" s="101" t="s">
+        <v>503</v>
       </c>
       <c r="C60" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Heat Extraction",</v>
+        <f t="shared" si="1"/>
+        <v>"O&amp;G" : "Oil and Gas Well Drilling",</v>
       </c>
       <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="G60" s="42"/>
+      <c r="H60"/>
     </row>
     <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B61" s="102" t="s">
-        <v>394</v>
+      <c r="A61" s="101" t="s">
+        <v>307</v>
+      </c>
+      <c r="B61" s="101" t="s">
+        <v>266</v>
       </c>
       <c r="C61" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Manufacturing",</v>
+        <f t="shared" si="1"/>
+        <v>"OTH" : "Other",</v>
       </c>
       <c r="D61" s="42"/>
+      <c r="E61" s="42"/>
+      <c r="G61" s="42"/>
+      <c r="H61"/>
     </row>
     <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B62" s="102" t="s">
-        <v>396</v>
+      <c r="A62" s="101" t="s">
+        <v>349</v>
+      </c>
+      <c r="B62" s="101" t="s">
+        <v>350</v>
       </c>
       <c r="C62" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Milling",</v>
+        <f t="shared" si="1"/>
+        <v>"OTH_CM" : "Other - Commercial",</v>
       </c>
       <c r="D62" s="42"/>
+      <c r="E62" s="42"/>
+      <c r="G62" s="42"/>
+      <c r="H62"/>
     </row>
     <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B63" s="102" t="s">
-        <v>398</v>
+      <c r="A63" s="101" t="s">
+        <v>364</v>
+      </c>
+      <c r="B63" s="101" t="s">
+        <v>365</v>
       </c>
       <c r="C63" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Mining",</v>
+        <f t="shared" si="1"/>
+        <v>"OTH_IN" : "Other - Industrial",</v>
       </c>
       <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
       <c r="G63" s="42"/>
       <c r="H63"/>
     </row>
     <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B64" s="102" t="s">
-        <v>400</v>
+      <c r="A64" s="101" t="s">
+        <v>389</v>
+      </c>
+      <c r="B64" s="101" t="s">
+        <v>390</v>
       </c>
       <c r="C64" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Other - Industrial",</v>
+        <f t="shared" si="1"/>
+        <v>"OTH_TM" : "Other - Temporary",</v>
       </c>
       <c r="D64" s="42"/>
+      <c r="E64" s="42"/>
       <c r="G64" s="42"/>
       <c r="H64"/>
     </row>
     <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B65" s="102" t="s">
-        <v>402</v>
+      <c r="A65" s="101" t="s">
+        <v>326</v>
+      </c>
+      <c r="B65" s="101" t="s">
+        <v>504</v>
       </c>
       <c r="C65" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Pollution Control",</v>
+        <f t="shared" si="1"/>
+        <v>"P&amp;S" : "Potable and Sanitary Supply",</v>
       </c>
       <c r="D65" s="42"/>
+      <c r="E65" s="42"/>
       <c r="G65" s="42"/>
       <c r="H65"/>
     </row>
     <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B66" s="102" t="s">
-        <v>404</v>
+      <c r="A66" s="101" t="s">
+        <v>366</v>
+      </c>
+      <c r="B66" s="101" t="s">
+        <v>367</v>
       </c>
       <c r="C66" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Power",</v>
+        <f t="shared" si="1"/>
+        <v>"PCT" : "Pollution Control",</v>
       </c>
       <c r="D66" s="42"/>
+      <c r="E66" s="42"/>
       <c r="G66" s="42"/>
       <c r="H66"/>
     </row>
     <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B67" s="102" t="s">
-        <v>406</v>
+      <c r="A67" s="101" t="s">
+        <v>368</v>
+      </c>
+      <c r="B67" s="101" t="s">
+        <v>369</v>
       </c>
       <c r="C67" s="42" t="str">
-        <f t="shared" si="0"/>
-        <v>"IND_SW" : "Refining",</v>
+        <f t="shared" si="1"/>
+        <v>"POW" : "Power",</v>
       </c>
       <c r="D67" s="42"/>
+      <c r="E67" s="42"/>
       <c r="G67" s="42"/>
       <c r="H67"/>
     </row>
     <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B68" s="102" t="s">
-        <v>408</v>
+      <c r="A68" s="101" t="s">
+        <v>308</v>
+      </c>
+      <c r="B68" s="101" t="s">
+        <v>267</v>
       </c>
       <c r="C68" s="42" t="str">
-        <f t="shared" ref="C68:C131" si="1">""""&amp;A68&amp;""""&amp;" : "&amp;""""&amp;B68&amp;""""&amp;","</f>
-        <v>"IND_SW" : "Reclamation Watering",</v>
+        <f t="shared" si="1"/>
+        <v>"RAI" : "Railroad",</v>
       </c>
       <c r="D68" s="42"/>
+      <c r="E68" s="42"/>
       <c r="G68" s="42"/>
       <c r="H68"/>
     </row>
     <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B69" s="102" t="s">
-        <v>410</v>
+      <c r="A69" s="101" t="s">
+        <v>391</v>
+      </c>
+      <c r="B69" s="101" t="s">
+        <v>392</v>
       </c>
       <c r="C69" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"IND_SW" : "Sediment Control",</v>
+        <v>"RDC" : "Road Construction",</v>
       </c>
       <c r="D69" s="42"/>
+      <c r="E69" s="42"/>
       <c r="G69" s="42"/>
       <c r="H69"/>
     </row>
     <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="102" t="s">
-        <v>319</v>
-      </c>
-      <c r="B70" s="102" t="s">
-        <v>412</v>
+      <c r="A70" s="101" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" s="101" t="s">
+        <v>268</v>
       </c>
       <c r="C70" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"IND_SW" : "Snow Making",</v>
+        <v>"REC" : "Recreation",</v>
       </c>
       <c r="D70" s="42"/>
+      <c r="E70" s="42"/>
       <c r="G70" s="42"/>
       <c r="H70"/>
     </row>
     <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="102" t="s">
-        <v>296</v>
-      </c>
-      <c r="B71" s="102" t="s">
-        <v>252</v>
+      <c r="A71" s="101" t="s">
+        <v>370</v>
+      </c>
+      <c r="B71" s="101" t="s">
+        <v>371</v>
       </c>
       <c r="C71" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"IRR_GW" : "Irrigation - ground water",</v>
+        <v>"REF" : "Refining",</v>
       </c>
       <c r="D71" s="42"/>
+      <c r="E71" s="42"/>
       <c r="G71" s="42"/>
       <c r="H71"/>
     </row>
     <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="102" t="s">
-        <v>320</v>
-      </c>
-      <c r="B72" s="102" t="s">
-        <v>276</v>
+      <c r="A72" s="101" t="s">
+        <v>310</v>
+      </c>
+      <c r="B72" s="101" t="s">
+        <v>269</v>
       </c>
       <c r="C72" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"IRR_SW" : "Irrigation - Surface water",</v>
+        <v>"RES" : "Reservoir Supply",</v>
       </c>
       <c r="D72" s="42"/>
+      <c r="E72" s="42"/>
       <c r="G72" s="42"/>
       <c r="H72"/>
     </row>
     <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="102" t="s">
-        <v>320</v>
-      </c>
-      <c r="B73" s="102" t="s">
-        <v>414</v>
+      <c r="A73" s="101" t="s">
+        <v>372</v>
+      </c>
+      <c r="B73" s="101" t="s">
+        <v>373</v>
       </c>
       <c r="C73" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"IRR_SW" : "Stock and/or Domestic",</v>
+        <v>"REW" : "Reclamation Watering",</v>
       </c>
       <c r="D73" s="42"/>
+      <c r="E73" s="42"/>
       <c r="G73" s="42"/>
       <c r="H73"/>
     </row>
     <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="102" t="s">
-        <v>321</v>
-      </c>
-      <c r="B74" s="102" t="s">
-        <v>277</v>
+      <c r="A74" s="101" t="s">
+        <v>327</v>
+      </c>
+      <c r="B74" s="101" t="s">
+        <v>505</v>
       </c>
       <c r="C74" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"ISF" : "Instream Flow - Only State of Wyo can apply",</v>
+        <v>"SDG" : "Gpm For Domestic or Stock",</v>
       </c>
       <c r="D74" s="42"/>
+      <c r="E74" s="42"/>
       <c r="G74" s="42"/>
       <c r="H74"/>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="102" t="s">
-        <v>322</v>
-      </c>
-      <c r="B75" s="102" t="s">
-        <v>278</v>
+      <c r="A75" s="101" t="s">
+        <v>378</v>
+      </c>
+      <c r="B75" s="101" t="s">
+        <v>506</v>
       </c>
       <c r="C75" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"LAK" : "Maintain Natural Lake Level (Phase II Award)",</v>
+        <v>"SDU" : "Stock and Domestic",</v>
       </c>
       <c r="D75" s="42"/>
+      <c r="E75" s="42"/>
       <c r="G75" s="42"/>
       <c r="H75"/>
     </row>
     <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="102" t="s">
-        <v>345</v>
-      </c>
-      <c r="B76" s="102" t="s">
-        <v>346</v>
+      <c r="A76" s="101" t="s">
+        <v>374</v>
+      </c>
+      <c r="B76" s="101" t="s">
+        <v>375</v>
       </c>
       <c r="C76" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"LAW" : "Large scale landscape",</v>
+        <v>"SED" : "Sediment Control",</v>
       </c>
       <c r="D76" s="42"/>
+      <c r="E76" s="42"/>
       <c r="G76" s="42"/>
       <c r="H76"/>
     </row>
     <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="102" t="s">
-        <v>375</v>
-      </c>
-      <c r="B77" s="102" t="s">
+      <c r="A77" s="101" t="s">
         <v>376</v>
+      </c>
+      <c r="B77" s="101" t="s">
+        <v>377</v>
       </c>
       <c r="C77" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MAI" : "Maintenance (Equipment Washing)",</v>
+        <v>"SNO" : "Snow Making",</v>
       </c>
       <c r="D77" s="42"/>
+      <c r="E77" s="42"/>
       <c r="G77" s="42"/>
       <c r="H77"/>
     </row>
     <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="102" t="s">
-        <v>393</v>
-      </c>
-      <c r="B78" s="102" t="s">
-        <v>394</v>
+      <c r="A78" s="101" t="s">
+        <v>311</v>
+      </c>
+      <c r="B78" s="101" t="s">
+        <v>270</v>
       </c>
       <c r="C78" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MAN" : "Manufacturing",</v>
+        <v>"STE" : "Stream",</v>
       </c>
       <c r="D78" s="42"/>
+      <c r="E78" s="42"/>
       <c r="G78" s="42"/>
       <c r="H78"/>
     </row>
     <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="102" t="s">
-        <v>377</v>
-      </c>
-      <c r="B79" s="102" t="s">
-        <v>378</v>
+      <c r="A79" s="101" t="s">
+        <v>282</v>
+      </c>
+      <c r="B79" s="101" t="s">
+        <v>251</v>
       </c>
       <c r="C79" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MEC" : "Mechanical ",</v>
+        <v>"STK" : "Stock Watering",</v>
       </c>
       <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
       <c r="G79" s="42"/>
       <c r="H79"/>
     </row>
     <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="102" t="s">
-        <v>379</v>
-      </c>
-      <c r="B80" s="102" t="s">
-        <v>380</v>
+      <c r="A80" s="101" t="s">
+        <v>312</v>
+      </c>
+      <c r="B80" s="101" t="s">
+        <v>271</v>
       </c>
       <c r="C80" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MED" : "Medicinal",</v>
+        <v>"STO" : "Stock",</v>
       </c>
       <c r="D80" s="42"/>
+      <c r="E80" s="42"/>
       <c r="G80" s="42"/>
       <c r="H80"/>
     </row>
     <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="102" t="s">
-        <v>424</v>
-      </c>
-      <c r="B81" s="102" t="s">
-        <v>425</v>
+      <c r="A81" s="101" t="s">
+        <v>393</v>
+      </c>
+      <c r="B81" s="101" t="s">
+        <v>251</v>
       </c>
       <c r="C81" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MEM" : "Municipal (Emergency)",</v>
+        <v>"STW" : "Stock Watering",</v>
       </c>
       <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
       <c r="G81" s="42"/>
       <c r="H81"/>
     </row>
     <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="102" t="s">
-        <v>395</v>
-      </c>
-      <c r="B82" s="102" t="s">
-        <v>396</v>
+      <c r="A82" s="101" t="s">
+        <v>328</v>
+      </c>
+      <c r="B82" s="101" t="s">
+        <v>507</v>
       </c>
       <c r="C82" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MIL" : "Milling",</v>
+        <v>"SWD" : "Subdivision",</v>
       </c>
       <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
       <c r="G82" s="42"/>
       <c r="H82"/>
     </row>
     <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="102" t="s">
-        <v>397</v>
-      </c>
-      <c r="B83" s="102" t="s">
-        <v>398</v>
+      <c r="A83" s="101" t="s">
+        <v>329</v>
+      </c>
+      <c r="B83" s="101" t="s">
+        <v>330</v>
       </c>
       <c r="C83" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MIN" : "Mining",</v>
+        <v>"SWP" : "Stock Water Pipeline",</v>
       </c>
       <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
       <c r="G83" s="42"/>
       <c r="H83"/>
     </row>
     <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="102" t="s">
-        <v>441</v>
-      </c>
-      <c r="B84" s="102" t="s">
-        <v>253</v>
+      <c r="A84" s="101" t="s">
+        <v>313</v>
+      </c>
+      <c r="B84" s="101" t="s">
+        <v>272</v>
       </c>
       <c r="C84" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MIS" : "Miscellaneous - ground water",</v>
+        <v>"TEM" : "Temporary",</v>
       </c>
       <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
       <c r="G84" s="42"/>
       <c r="H84"/>
     </row>
     <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="102" t="s">
-        <v>297</v>
-      </c>
-      <c r="B85" s="102" t="s">
-        <v>362</v>
+      <c r="A85" s="101" t="s">
+        <v>314</v>
+      </c>
+      <c r="B85" s="101" t="s">
+        <v>482</v>
       </c>
       <c r="C85" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MON" : "Monitor, Observation",</v>
+        <v>"TENL" : "Total Enlargement",</v>
       </c>
       <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
       <c r="G85" s="42"/>
       <c r="H85"/>
     </row>
     <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="102" t="s">
-        <v>298</v>
-      </c>
-      <c r="B86" s="102" t="s">
-        <v>254</v>
+      <c r="A86" s="101" t="s">
+        <v>315</v>
+      </c>
+      <c r="B86" s="101" t="s">
+        <v>273</v>
       </c>
       <c r="C86" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MUN_GW" : "Municipal - ground water",</v>
+        <v>"TRA" : "Transportation",</v>
       </c>
       <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
       <c r="G86" s="42"/>
       <c r="H86"/>
     </row>
     <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="102" t="s">
-        <v>323</v>
-      </c>
-      <c r="B87" s="102" t="s">
-        <v>279</v>
+      <c r="A87" s="101" t="s">
+        <v>283</v>
+      </c>
+      <c r="B87" s="101" t="s">
+        <v>252</v>
       </c>
       <c r="C87" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"MUN_SW" : "Municipal - Surface water",</v>
+        <v>"TST" : "Test Well",</v>
       </c>
       <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
       <c r="G87" s="42"/>
       <c r="H87"/>
     </row>
     <row r="88" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A88" s="102" t="s">
-        <v>324</v>
-      </c>
-      <c r="B88" s="102" t="s">
-        <v>280</v>
+      <c r="A88" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="B88" s="101" t="s">
+        <v>508</v>
       </c>
       <c r="C88" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"NAT" : "Natural Flow (Phase II Award)",</v>
+        <v>"TWR" : "Tree Watering",</v>
       </c>
       <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
       <c r="G88" s="42"/>
       <c r="H88"/>
     </row>
     <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A89" s="102" t="s">
-        <v>347</v>
-      </c>
-      <c r="B89" s="102" t="s">
-        <v>348</v>
+      <c r="A89" s="101" t="s">
+        <v>316</v>
+      </c>
+      <c r="B89" s="101" t="s">
+        <v>274</v>
       </c>
       <c r="C89" s="42" t="str">
         <f t="shared" si="1"/>
-        <v>"O&amp;G" : "Oil &amp; Gas well drilling",</v>
+        <v>"UTL" : "Utilities",</v>
       </c>
       <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
       <c r="G89" s="42"/>
       <c r="H89"/>
     </row>
     <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A90" s="102" t="s">
-        <v>325</v>
-      </c>
-      <c r="B90" s="102" t="s">
-        <v>281</v>
+      <c r="A90" s="101" t="s">
+        <v>317</v>
+      </c>
+      <c r="B90" s="101" t="s">
+        <v>509</v>
       </c>
       <c r="C90" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"OTH" : "Other",</v>
+        <f t="shared" ref="C90:C94" si="2">""""&amp;A90&amp;""""&amp;" : "&amp;""""&amp;B90&amp;""""&amp;","</f>
+        <v>"W&amp;S" : "Wild and Scenic",</v>
       </c>
       <c r="D90" s="42"/>
+      <c r="E90" s="42"/>
       <c r="G90" s="42"/>
       <c r="H90"/>
     </row>
     <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="102" t="s">
-        <v>325</v>
-      </c>
-      <c r="B91" s="102" t="s">
-        <v>349</v>
+      <c r="A91" s="101" t="s">
+        <v>395</v>
+      </c>
+      <c r="B91" s="101" t="s">
+        <v>396</v>
       </c>
       <c r="C91" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"OTH" : "Others",</v>
+        <f t="shared" si="2"/>
+        <v>"WDR" : "Well Drilling",</v>
       </c>
       <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
       <c r="G91" s="42"/>
       <c r="H91"/>
     </row>
     <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="102" t="s">
-        <v>381</v>
-      </c>
-      <c r="B92" s="102" t="s">
-        <v>382</v>
+      <c r="A92" s="101" t="s">
+        <v>318</v>
+      </c>
+      <c r="B92" s="101" t="s">
+        <v>275</v>
       </c>
       <c r="C92" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"OTH_CM" : "Other - Commercial",</v>
+        <f t="shared" si="2"/>
+        <v>"WET" : "Wetlands",</v>
       </c>
       <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
       <c r="G92" s="42"/>
       <c r="H92"/>
     </row>
     <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="102" t="s">
-        <v>399</v>
-      </c>
-      <c r="B93" s="102" t="s">
-        <v>400</v>
+      <c r="A93" s="101" t="s">
+        <v>331</v>
+      </c>
+      <c r="B93" s="101" t="s">
+        <v>510</v>
       </c>
       <c r="C93" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"OTH_IN" : "Other - Industrial",</v>
+        <f t="shared" si="2"/>
+        <v>"WHL" : "Water Hauls",</v>
       </c>
       <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
       <c r="G93" s="42"/>
       <c r="H93"/>
     </row>
     <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A94" s="102" t="s">
-        <v>426</v>
-      </c>
-      <c r="B94" s="102" t="s">
-        <v>427</v>
+      <c r="A94" s="101" t="s">
+        <v>319</v>
+      </c>
+      <c r="B94" s="101" t="s">
+        <v>250</v>
       </c>
       <c r="C94" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"OTH_TM" : "Other - Temporary",</v>
+        <f t="shared" si="2"/>
+        <v>"WL" : "Wildlife",</v>
       </c>
       <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
       <c r="G94" s="42"/>
       <c r="H94"/>
     </row>
-    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="102" t="s">
-        <v>350</v>
-      </c>
-      <c r="B95" s="102" t="s">
-        <v>351</v>
-      </c>
-      <c r="C95" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"P&amp;S" : "Potable &amp; Sanitary Supply",</v>
-      </c>
-      <c r="D95" s="42"/>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="102"/>
+      <c r="B95" s="102"/>
       <c r="G95" s="42"/>
       <c r="H95"/>
     </row>
-    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="102" t="s">
-        <v>401</v>
-      </c>
-      <c r="B96" s="102" t="s">
-        <v>402</v>
-      </c>
-      <c r="C96" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"PCT" : "Pollution Control",</v>
-      </c>
-      <c r="D96" s="42"/>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="102"/>
+      <c r="B96" s="102"/>
       <c r="G96" s="42"/>
       <c r="H96"/>
     </row>
-    <row r="97" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A97" s="102" t="s">
-        <v>403</v>
-      </c>
-      <c r="B97" s="102" t="s">
-        <v>404</v>
-      </c>
-      <c r="C97" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"POW" : "Power",</v>
-      </c>
-      <c r="D97" s="42"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="102"/>
+      <c r="B97" s="102"/>
       <c r="G97" s="42"/>
       <c r="H97"/>
     </row>
-    <row r="98" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="102" t="s">
-        <v>326</v>
-      </c>
-      <c r="B98" s="102" t="s">
-        <v>282</v>
-      </c>
-      <c r="C98" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"RAI" : "Railroad",</v>
-      </c>
-      <c r="D98" s="42"/>
-      <c r="G98" s="42"/>
-      <c r="H98"/>
-    </row>
-    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="102" t="s">
-        <v>428</v>
-      </c>
-      <c r="B99" s="102" t="s">
-        <v>429</v>
-      </c>
-      <c r="C99" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"RDC" : "Road Construction",</v>
-      </c>
-      <c r="D99" s="42"/>
-      <c r="G99" s="42"/>
-      <c r="H99"/>
-    </row>
-    <row r="100" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="102" t="s">
-        <v>327</v>
-      </c>
-      <c r="B100" s="102" t="s">
-        <v>283</v>
-      </c>
-      <c r="C100" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"REC" : "Recreation",</v>
-      </c>
-      <c r="D100" s="42"/>
-      <c r="G100" s="42"/>
-      <c r="H100"/>
-    </row>
-    <row r="101" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="102" t="s">
-        <v>327</v>
-      </c>
-      <c r="B101" s="102" t="s">
-        <v>416</v>
-      </c>
-      <c r="C101" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"REC" : "Recreation (Aesthetics)",</v>
-      </c>
-      <c r="D101" s="42"/>
-      <c r="G101" s="42"/>
-      <c r="H101"/>
-    </row>
-    <row r="102" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A102" s="102" t="s">
-        <v>405</v>
-      </c>
-      <c r="B102" s="102" t="s">
-        <v>406</v>
-      </c>
-      <c r="C102" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"REF" : "Refining",</v>
-      </c>
-      <c r="D102" s="42"/>
-      <c r="G102" s="42"/>
-      <c r="H102"/>
-    </row>
-    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="102" t="s">
-        <v>328</v>
-      </c>
-      <c r="B103" s="102" t="s">
-        <v>284</v>
-      </c>
-      <c r="C103" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"RES" : "Reservoir Supply",</v>
-      </c>
-      <c r="D103" s="42"/>
-      <c r="G103" s="42"/>
-      <c r="H103"/>
-    </row>
-    <row r="104" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A104" s="102" t="s">
-        <v>407</v>
-      </c>
-      <c r="B104" s="102" t="s">
-        <v>408</v>
-      </c>
-      <c r="C104" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"REW" : "Reclamation Watering",</v>
-      </c>
-      <c r="D104" s="42"/>
-      <c r="G104" s="42"/>
-      <c r="H104"/>
-    </row>
-    <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A105" s="102" t="s">
-        <v>352</v>
-      </c>
-      <c r="B105" s="102" t="s">
-        <v>353</v>
-      </c>
-      <c r="C105" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SDG" : "&gt; gpm for Domestic &amp;/or stock",</v>
-      </c>
-      <c r="D105" s="42"/>
-      <c r="G105" s="42"/>
-      <c r="H105"/>
-    </row>
-    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="102" t="s">
-        <v>413</v>
-      </c>
-      <c r="B106" s="102" t="s">
-        <v>414</v>
-      </c>
-      <c r="C106" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SDU" : "Stock and/or Domestic",</v>
-      </c>
-      <c r="D106" s="42"/>
-      <c r="G106" s="42"/>
-      <c r="H106"/>
-    </row>
-    <row r="107" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A107" s="102" t="s">
-        <v>409</v>
-      </c>
-      <c r="B107" s="102" t="s">
-        <v>410</v>
-      </c>
-      <c r="C107" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SED" : "Sediment Control",</v>
-      </c>
-      <c r="D107" s="42"/>
-      <c r="G107" s="42"/>
-      <c r="H107"/>
-    </row>
-    <row r="108" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A108" s="102" t="s">
-        <v>411</v>
-      </c>
-      <c r="B108" s="102" t="s">
-        <v>412</v>
-      </c>
-      <c r="C108" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SNO" : "Snow Making",</v>
-      </c>
-      <c r="D108" s="42"/>
-      <c r="G108" s="42"/>
-      <c r="H108"/>
-    </row>
-    <row r="109" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="102" t="s">
-        <v>329</v>
-      </c>
-      <c r="B109" s="102" t="s">
-        <v>285</v>
-      </c>
-      <c r="C109" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STE" : "Stream",</v>
-      </c>
-      <c r="D109" s="42"/>
-      <c r="G109" s="42"/>
-      <c r="H109"/>
-    </row>
-    <row r="110" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="102" t="s">
-        <v>299</v>
-      </c>
-      <c r="B110" s="102" t="s">
-        <v>255</v>
-      </c>
-      <c r="C110" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STK" : "Stock Watering",</v>
-      </c>
-      <c r="D110" s="42"/>
-      <c r="G110" s="42"/>
-      <c r="H110"/>
-    </row>
-    <row r="111" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="102" t="s">
-        <v>299</v>
-      </c>
-      <c r="B111" s="102" t="s">
-        <v>383</v>
-      </c>
-      <c r="C111" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STK" : "Stockyard (Pig, Cow, Chicken)",</v>
-      </c>
-      <c r="D111" s="42"/>
-      <c r="G111" s="42"/>
-      <c r="H111"/>
-    </row>
-    <row r="112" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A112" s="102" t="s">
-        <v>330</v>
-      </c>
-      <c r="B112" s="102" t="s">
-        <v>286</v>
-      </c>
-      <c r="C112" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STO" : "Stock",</v>
-      </c>
-      <c r="D112" s="42"/>
-      <c r="G112" s="42"/>
-      <c r="H112"/>
-    </row>
-    <row r="113" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="102" t="s">
-        <v>330</v>
-      </c>
-      <c r="B113" s="102" t="s">
-        <v>418</v>
-      </c>
-      <c r="C113" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STO" : "Stock (Aesthetics)",</v>
-      </c>
-      <c r="D113" s="42"/>
-      <c r="G113" s="42"/>
-      <c r="H113"/>
-    </row>
-    <row r="114" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A114" s="102" t="s">
-        <v>430</v>
-      </c>
-      <c r="B114" s="102" t="s">
-        <v>431</v>
-      </c>
-      <c r="C114" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"STW" : "Stock watering",</v>
-      </c>
-      <c r="D114" s="42"/>
-      <c r="G114" s="42"/>
-      <c r="H114"/>
-    </row>
-    <row r="115" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A115" s="102" t="s">
-        <v>354</v>
-      </c>
-      <c r="B115" s="102" t="s">
-        <v>355</v>
-      </c>
-      <c r="C115" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SWD" : "Subdivison, water districts, etc",</v>
-      </c>
-      <c r="D115" s="42"/>
-      <c r="G115" s="42"/>
-      <c r="H115"/>
-    </row>
-    <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="102" t="s">
-        <v>356</v>
-      </c>
-      <c r="B116" s="102" t="s">
-        <v>357</v>
-      </c>
-      <c r="C116" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"SWP" : "Stock Water Pipeline",</v>
-      </c>
-      <c r="D116" s="42"/>
-      <c r="G116" s="42"/>
-      <c r="H116"/>
-    </row>
-    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A117" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B117" s="102" t="s">
-        <v>287</v>
-      </c>
-      <c r="C117" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Temporary",</v>
-      </c>
-      <c r="D117" s="42"/>
-      <c r="G117" s="42"/>
-      <c r="H117"/>
-    </row>
-    <row r="118" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A118" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B118" s="102" t="s">
-        <v>419</v>
-      </c>
-      <c r="C118" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Construction",</v>
-      </c>
-      <c r="D118" s="42"/>
-      <c r="G118" s="42"/>
-      <c r="H118"/>
-    </row>
-    <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A119" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B119" s="102" t="s">
-        <v>421</v>
-      </c>
-      <c r="C119" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Dust Abatement",</v>
-      </c>
-      <c r="D119" s="42"/>
-      <c r="G119" s="42"/>
-      <c r="H119"/>
-    </row>
-    <row r="120" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A120" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B120" s="102" t="s">
-        <v>423</v>
-      </c>
-      <c r="C120" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Hydrostatic Testing",</v>
-      </c>
-      <c r="D120" s="42"/>
-      <c r="G120" s="42"/>
-      <c r="H120"/>
-    </row>
-    <row r="121" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B121" s="102" t="s">
-        <v>425</v>
-      </c>
-      <c r="C121" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Municipal (Emergency)",</v>
-      </c>
-      <c r="D121" s="42"/>
-      <c r="G121" s="42"/>
-      <c r="H121"/>
-    </row>
-    <row r="122" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B122" s="102" t="s">
-        <v>427</v>
-      </c>
-      <c r="C122" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Other - Temporary",</v>
-      </c>
-      <c r="D122" s="42"/>
-      <c r="G122" s="42"/>
-      <c r="H122"/>
-    </row>
-    <row r="123" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A123" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B123" s="102" t="s">
-        <v>429</v>
-      </c>
-      <c r="C123" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Road Construction",</v>
-      </c>
-      <c r="D123" s="42"/>
-      <c r="G123" s="42"/>
-      <c r="H123"/>
-    </row>
-    <row r="124" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B124" s="102" t="s">
-        <v>431</v>
-      </c>
-      <c r="C124" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Stock watering",</v>
-      </c>
-      <c r="D124" s="42"/>
-      <c r="G124" s="42"/>
-      <c r="H124"/>
-    </row>
-    <row r="125" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B125" s="102" t="s">
-        <v>433</v>
-      </c>
-      <c r="C125" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Tree watering (non-commercial)",</v>
-      </c>
-      <c r="D125" s="42"/>
-      <c r="G125" s="42"/>
-      <c r="H125"/>
-    </row>
-    <row r="126" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="102" t="s">
-        <v>331</v>
-      </c>
-      <c r="B126" s="102" t="s">
-        <v>435</v>
-      </c>
-      <c r="C126" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TEM" : "Well Drilling",</v>
-      </c>
-      <c r="D126" s="42"/>
-      <c r="G126" s="42"/>
-      <c r="H126"/>
-    </row>
-    <row r="127" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A127" s="102" t="s">
-        <v>332</v>
-      </c>
-      <c r="B127" s="102" t="s">
-        <v>288</v>
-      </c>
-      <c r="C127" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TENL" : "Total Enlargement for this application",</v>
-      </c>
-      <c r="D127" s="42"/>
-      <c r="G127" s="42"/>
-      <c r="H127"/>
-    </row>
-    <row r="128" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A128" s="102" t="s">
-        <v>333</v>
-      </c>
-      <c r="B128" s="102" t="s">
-        <v>289</v>
-      </c>
-      <c r="C128" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TRA" : "Transportation",</v>
-      </c>
-      <c r="D128" s="42"/>
-      <c r="G128" s="42"/>
-      <c r="H128"/>
-    </row>
-    <row r="129" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A129" s="102" t="s">
-        <v>300</v>
-      </c>
-      <c r="B129" s="102" t="s">
-        <v>256</v>
-      </c>
-      <c r="C129" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TST" : "Test Well",</v>
-      </c>
-      <c r="D129" s="42"/>
-      <c r="G129" s="42"/>
-      <c r="H129"/>
-    </row>
-    <row r="130" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="102" t="s">
-        <v>432</v>
-      </c>
-      <c r="B130" s="102" t="s">
-        <v>433</v>
-      </c>
-      <c r="C130" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"TWR" : "Tree watering (non-commercial)",</v>
-      </c>
-      <c r="D130" s="42"/>
-      <c r="G130" s="42"/>
-      <c r="H130"/>
-    </row>
-    <row r="131" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A131" s="102" t="s">
-        <v>334</v>
-      </c>
-      <c r="B131" s="102" t="s">
-        <v>290</v>
-      </c>
-      <c r="C131" s="42" t="str">
-        <f t="shared" si="1"/>
-        <v>"UTL" : "Utilities",</v>
-      </c>
-      <c r="D131" s="42"/>
-      <c r="G131" s="42"/>
-      <c r="H131"/>
-    </row>
-    <row r="132" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" s="102" t="s">
-        <v>335</v>
-      </c>
-      <c r="B132" s="102" t="s">
-        <v>291</v>
-      </c>
-      <c r="C132" s="42" t="str">
-        <f t="shared" ref="C132:C138" si="2">""""&amp;A132&amp;""""&amp;" : "&amp;""""&amp;B132&amp;""""&amp;","</f>
-        <v>"W&amp;S" : "Wild &amp; Scenic - only State of Wyo can apply",</v>
-      </c>
-      <c r="D132" s="42"/>
-      <c r="G132" s="42"/>
-      <c r="H132"/>
-    </row>
-    <row r="133" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="102" t="s">
-        <v>434</v>
-      </c>
-      <c r="B133" s="102" t="s">
-        <v>435</v>
-      </c>
-      <c r="C133" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WDR" : "Well Drilling",</v>
-      </c>
-      <c r="D133" s="42"/>
-      <c r="G133" s="42"/>
-      <c r="H133"/>
-    </row>
-    <row r="134" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="102" t="s">
-        <v>336</v>
-      </c>
-      <c r="B134" s="102" t="s">
-        <v>292</v>
-      </c>
-      <c r="C134" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WET" : "Wetlands",</v>
-      </c>
-      <c r="D134" s="42"/>
-      <c r="G134" s="42"/>
-      <c r="H134"/>
-    </row>
-    <row r="135" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A135" s="102" t="s">
-        <v>336</v>
-      </c>
-      <c r="B135" s="102" t="s">
-        <v>437</v>
-      </c>
-      <c r="C135" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WET" : "Wetlands (Aesthetics)",</v>
-      </c>
-      <c r="D135" s="42"/>
-      <c r="G135" s="42"/>
-      <c r="H135"/>
-    </row>
-    <row r="136" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A136" s="102" t="s">
-        <v>358</v>
-      </c>
-      <c r="B136" s="102" t="s">
-        <v>359</v>
-      </c>
-      <c r="C136" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WHL" : "Water hauls",</v>
-      </c>
-      <c r="D136" s="42"/>
-      <c r="G136" s="42"/>
-      <c r="H136"/>
-    </row>
-    <row r="137" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A137" s="102" t="s">
-        <v>337</v>
-      </c>
-      <c r="B137" s="102" t="s">
-        <v>250</v>
-      </c>
-      <c r="C137" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WL" : "Wildlife",</v>
-      </c>
-      <c r="D137" s="42"/>
-      <c r="G137" s="42"/>
-      <c r="H137"/>
-    </row>
-    <row r="138" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A138" s="102" t="s">
-        <v>337</v>
-      </c>
-      <c r="B138" s="102" t="s">
-        <v>439</v>
-      </c>
-      <c r="C138" s="42" t="str">
-        <f t="shared" si="2"/>
-        <v>"WL" : "Wildlife (Aesthetics)",</v>
-      </c>
-      <c r="D138" s="42"/>
-      <c r="G138" s="42"/>
-      <c r="H138"/>
-    </row>
-    <row r="139" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A139" s="99"/>
-      <c r="B139" s="99"/>
-      <c r="G139" s="42"/>
-      <c r="H139"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="103"/>
-      <c r="B140" s="103"/>
-      <c r="G140" s="42"/>
-      <c r="H140"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A141" s="103"/>
-      <c r="B141" s="103"/>
-      <c r="G141" s="42"/>
-      <c r="H141"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A142" s="103"/>
-      <c r="B142" s="103"/>
-      <c r="G142" s="42"/>
-      <c r="H142"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A143" s="103"/>
-      <c r="B143" s="103"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A144" s="103"/>
-      <c r="B144" s="103"/>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="102"/>
+      <c r="B98" s="102"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="102"/>
+      <c r="B99" s="102"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B144">
-    <sortCondition ref="A3:A144"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B99">
+    <sortCondition ref="A3:A99"/>
   </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
WY water rights update.
WY water rights update.
</commit_message>
<xml_diff>
--- a/Wyoming/WaterAllocation/WY_Allocation Schema Mapping to WaDE_QA.xlsx
+++ b/Wyoming/WaterAllocation/WY_Allocation Schema Mapping to WaDE_QA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjame\Documents\WSWC Documents\MappingStatesDataToWaDE2.0\Wyoming\WaterAllocation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6268B78-F310-45A0-AD50-45AF9143D52E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C7E244-0844-47BE-94E5-F1A3910FAB23}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="7" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="714" activeTab="8" xr2:uid="{10FC1BAB-5472-410C-A2F0-85DCDF5389F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping Notes" sheetId="10" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Sites" sheetId="5" r:id="rId6"/>
     <sheet name="AllocationsAmounts_fact" sheetId="7" r:id="rId7"/>
     <sheet name="WY_dictionaries" sheetId="9" r:id="rId8"/>
+    <sheet name="missing ben uses" sheetId="11" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="516">
   <si>
     <t>Name</t>
   </si>
@@ -1595,6 +1596,24 @@
   </si>
   <si>
     <t>Water Hauls</t>
+  </si>
+  <si>
+    <t>Uses</t>
+  </si>
+  <si>
+    <t>MIS_SW</t>
+  </si>
+  <si>
+    <t>S&amp;D</t>
+  </si>
+  <si>
+    <t>STS</t>
+  </si>
+  <si>
+    <t>STKNDMS</t>
+  </si>
+  <si>
+    <t>OIL</t>
   </si>
 </sst>
 </file>
@@ -2446,7 +2465,7 @@
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2779,6 +2798,8 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5460,8 +5481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91B1FF-D207-4871-B787-27544A9D3030}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6924,8 +6945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A68CD9-E6C8-4C1E-8A36-F76F66BA5935}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A64" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8492,4 +8513,273 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A4D730E-5938-430B-ADEE-1D881E5D0F28}">
+  <dimension ref="A1:H46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="114" t="s">
+        <v>510</v>
+      </c>
+      <c r="E1" s="114"/>
+      <c r="H1" s="114"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="115" t="s">
+        <v>511</v>
+      </c>
+      <c r="B41" s="115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="115" t="s">
+        <v>515</v>
+      </c>
+      <c r="B42" s="115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="115" t="s">
+        <v>512</v>
+      </c>
+      <c r="B43" s="115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="115" t="s">
+        <v>514</v>
+      </c>
+      <c r="B44" s="115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="115" t="s">
+        <v>513</v>
+      </c>
+      <c r="B45" s="115" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="115"/>
+      <c r="B46" s="115"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2330">
+    <sortCondition ref="B2:B2330"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>